<commit_message>
small changes to script and readme associated with revisions
</commit_message>
<xml_diff>
--- a/outputs/OutputsEstimates.xlsx
+++ b/outputs/OutputsEstimates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ian/Dropbox/Dworkin_lab/DukasDworkinLabShared/CB_RD_Manuscript_2021/outputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ian/Dropbox/Dworkin_lab/DukasDworkinLabShared/CB_RD_Aggression2022/outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C66F82-417C-BC43-AE90-9A3184634233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B0957A-1C1C-6148-9BE1-32C70DC76408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9360" yWindow="500" windowWidth="38420" windowHeight="24220" xr2:uid="{8C6C77C8-D291-7F4C-8F86-0B8A216DDF10}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{8C6C77C8-D291-7F4C-8F86-0B8A216DDF10}"/>
   </bookViews>
   <sheets>
     <sheet name="model_outputs" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="43">
   <si>
     <t>Male only aggression</t>
   </si>
@@ -152,6 +151,18 @@
   </si>
   <si>
     <t>AIC restricted model (single genetic variance term)</t>
+  </si>
+  <si>
+    <t>approximate 95%CIs on ratio (lower, upper)</t>
+  </si>
+  <si>
+    <t>lower</t>
+  </si>
+  <si>
+    <t>upper</t>
+  </si>
+  <si>
+    <t>calculated on log difference, and exponentiated</t>
   </si>
 </sst>
 </file>
@@ -531,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2812776-5E37-0F43-88FD-34BC202C5C1D}">
-  <dimension ref="A1:O45"/>
+  <dimension ref="A1:O48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -921,352 +932,395 @@
         <v>31</v>
       </c>
     </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" t="s">
+        <v>41</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L20" t="s">
+        <v>40</v>
+      </c>
+      <c r="M20" t="s">
+        <v>41</v>
+      </c>
+    </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21">
+        <v>0.89</v>
+      </c>
+      <c r="D21">
+        <v>1.55</v>
+      </c>
+      <c r="J21" t="s">
+        <v>42</v>
+      </c>
+      <c r="L21">
+        <v>0.189</v>
+      </c>
+      <c r="M21">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
         <v>9</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C25" t="s">
         <v>16</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D25" t="s">
         <v>17</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K25" t="s">
         <v>9</v>
       </c>
-      <c r="L22" t="s">
+      <c r="L25" t="s">
         <v>16</v>
       </c>
-      <c r="M22" t="s">
+      <c r="M25" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B26" s="3">
         <v>0.74</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C26" s="3">
         <v>0.25</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D26" s="3">
         <v>0.89</v>
       </c>
-      <c r="J23" s="3" t="s">
+      <c r="J26" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K23" s="3">
+      <c r="K26" s="3">
         <v>0.78700000000000003</v>
       </c>
-      <c r="L23" s="3">
+      <c r="L26" s="3">
         <v>0.11600000000000001</v>
       </c>
-      <c r="M23" s="3">
+      <c r="M26" s="3">
         <v>0.92500000000000004</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>18</v>
-      </c>
-      <c r="B24">
-        <v>0.79</v>
-      </c>
-      <c r="C24">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="D24">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="J24" t="s">
-        <v>18</v>
-      </c>
-      <c r="K24">
-        <v>0.80559999999999998</v>
-      </c>
-      <c r="L24">
-        <v>0.50329999999999997</v>
-      </c>
-      <c r="M24">
-        <v>1.29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25">
-        <v>0.52600000000000002</v>
-      </c>
-      <c r="C25">
-        <v>0.36699999999999999</v>
-      </c>
-      <c r="D25">
-        <v>0.75</v>
-      </c>
-      <c r="J25" t="s">
-        <v>19</v>
-      </c>
-      <c r="K25">
-        <v>0.80720000000000003</v>
-      </c>
-      <c r="L25">
-        <v>0.50800000000000001</v>
-      </c>
-      <c r="M25">
-        <v>1.28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26">
-        <v>0.45</v>
-      </c>
-      <c r="C26">
-        <v>0.27800000000000002</v>
-      </c>
-      <c r="D26">
-        <v>0.58199999999999996</v>
-      </c>
-      <c r="J26" t="s">
-        <v>21</v>
-      </c>
-      <c r="K26">
-        <v>0.79769999999999996</v>
-      </c>
-      <c r="L26">
-        <v>0.69699999999999995</v>
-      </c>
-      <c r="M26">
-        <v>0.85799999999999998</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B27">
-        <v>1.18</v>
+        <v>0.79</v>
       </c>
       <c r="C27">
-        <v>1.01</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="D27">
-        <v>1.38</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="J27" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="K27">
-        <v>1.81</v>
+        <v>0.80559999999999998</v>
       </c>
       <c r="L27">
-        <v>1.56</v>
+        <v>0.50329999999999997</v>
       </c>
       <c r="M27">
-        <v>2.1</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28">
+        <v>0.52600000000000002</v>
+      </c>
+      <c r="C28">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="D28">
+        <v>0.75</v>
+      </c>
+      <c r="J28" t="s">
+        <v>19</v>
+      </c>
+      <c r="K28">
+        <v>0.80720000000000003</v>
+      </c>
+      <c r="L28">
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="M28">
+        <v>1.28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29">
+        <v>0.45</v>
+      </c>
+      <c r="C29">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="D29">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="J29" t="s">
+        <v>21</v>
+      </c>
+      <c r="K29">
+        <v>0.79769999999999996</v>
+      </c>
+      <c r="L29">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="M29">
+        <v>0.85799999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30">
+        <v>1.18</v>
+      </c>
+      <c r="C30">
+        <v>1.01</v>
+      </c>
+      <c r="D30">
+        <v>1.38</v>
+      </c>
+      <c r="J30" t="s">
+        <v>22</v>
+      </c>
+      <c r="K30">
+        <v>1.81</v>
+      </c>
+      <c r="L30">
+        <v>1.56</v>
+      </c>
+      <c r="M30">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>23</v>
       </c>
-      <c r="B28">
+      <c r="B31">
         <v>0.80100000000000005</v>
       </c>
-      <c r="C28">
+      <c r="C31">
         <v>0.67600000000000005</v>
       </c>
-      <c r="D28">
+      <c r="D31">
         <v>0.95</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J31" t="s">
         <v>23</v>
       </c>
-      <c r="K28">
+      <c r="K31">
         <v>1.85</v>
       </c>
-      <c r="L28">
+      <c r="L31">
         <v>1.64</v>
       </c>
-      <c r="M28">
+      <c r="M31">
         <v>2.09</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B30" s="1" t="s">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="K30" s="1" t="s">
+      <c r="K33" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J31" s="2" t="s">
+      <c r="J34" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
         <v>26</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C35" t="s">
         <v>3</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D35" t="s">
         <v>27</v>
       </c>
-      <c r="K32" t="s">
+      <c r="K35" t="s">
         <v>26</v>
       </c>
-      <c r="L32" t="s">
+      <c r="L35" t="s">
         <v>3</v>
       </c>
-      <c r="M32" t="s">
+      <c r="M35" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B33">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B36">
         <v>14.2</v>
       </c>
-      <c r="C33">
+      <c r="C36">
         <v>1</v>
       </c>
-      <c r="D33">
+      <c r="D36">
         <v>1.6000000000000001E-4</v>
       </c>
-      <c r="K33">
+      <c r="K36">
         <v>8.75</v>
       </c>
-      <c r="L33">
+      <c r="L36">
         <v>1</v>
       </c>
-      <c r="M33">
+      <c r="M36">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>28</v>
       </c>
-      <c r="B34">
+      <c r="B37">
         <v>3111</v>
       </c>
-      <c r="J34" t="s">
+      <c r="J37" t="s">
         <v>28</v>
       </c>
-      <c r="K34">
+      <c r="K37">
         <v>2186</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>29</v>
       </c>
-      <c r="B35">
+      <c r="B38">
         <v>3124</v>
       </c>
-      <c r="J35" t="s">
+      <c r="J38" t="s">
         <v>29</v>
       </c>
-      <c r="K35">
+      <c r="K38">
         <v>2193</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J37" s="2" t="s">
+      <c r="J40" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
         <v>26</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C41" t="s">
         <v>3</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D41" t="s">
         <v>27</v>
       </c>
-      <c r="K38" t="s">
+      <c r="K41" t="s">
         <v>26</v>
       </c>
-      <c r="L38" t="s">
+      <c r="L41" t="s">
         <v>3</v>
       </c>
-      <c r="M38" t="s">
+      <c r="M41" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B39">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B42">
         <v>25.56</v>
       </c>
-      <c r="C39">
+      <c r="C42">
         <v>2</v>
       </c>
-      <c r="D39">
+      <c r="D42">
         <v>8.1999999999999998E-4</v>
       </c>
-      <c r="K39">
+      <c r="K42">
         <v>11.71</v>
       </c>
-      <c r="L39">
+      <c r="L42">
         <v>2</v>
       </c>
-      <c r="M39">
+      <c r="M42">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>28</v>
       </c>
-      <c r="B40">
+      <c r="B43">
         <v>3111</v>
       </c>
-      <c r="J40" t="s">
+      <c r="J43" t="s">
         <v>28</v>
       </c>
-      <c r="K40">
+      <c r="K43">
         <v>2186</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>38</v>
       </c>
-      <c r="B41">
+      <c r="B44">
         <v>3133</v>
       </c>
-      <c r="J41" t="s">
+      <c r="J44" t="s">
         <v>38</v>
       </c>
-      <c r="K41">
+      <c r="K44">
         <v>2194</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>